<commit_message>
platform doc and database export
export done to match everyones
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_1_SprintBacklog_1.xlsx
+++ b/documents/FlyingMongeese_Deliverable_1_SprintBacklog_1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="22740" windowHeight="15560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="22740" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SprintBacklog1" sheetId="2" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -294,15 +294,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -628,26 +620,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="A1:K12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -679,7 +671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>10</v>
       </c>
@@ -710,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>11</v>
       </c>
@@ -741,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="91" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>12</v>
       </c>
@@ -771,7 +763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>13</v>
       </c>
@@ -801,7 +793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>14</v>
       </c>
@@ -830,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>15</v>
       </c>
@@ -844,7 +836,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>37</v>
@@ -862,7 +854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>16</v>
       </c>
@@ -894,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>17</v>
       </c>
@@ -927,7 +919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>18</v>
       </c>
@@ -957,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>19</v>
       </c>
@@ -987,400 +979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="78" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
-        <v>20</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="169" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
-        <v>10</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="156" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
-        <v>11</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="195" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="143" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="169" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="156" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>15</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="156" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
-        <v>16</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="143" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
-        <v>17</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="130" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>18</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="143" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>19</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="130" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>20</v>
       </c>
@@ -1423,24 +1022,421 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>20</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView topLeftCell="E8" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="58.6640625" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1472,7 +1468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="76" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1497,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1522,7 +1518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1545,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1568,7 +1564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1591,7 +1587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1614,7 +1610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1664,7 +1660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1687,7 +1683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1710,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1760,7 +1756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="78" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1783,37 +1779,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="6:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="6:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="6:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="6:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="6:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>

</xml_diff>